<commit_message>
corregir calificacion D7 estudiantes
</commit_message>
<xml_diff>
--- a/utils/cleaners/Marco_consolidacion/Dimensión 1.xlsx
+++ b/utils/cleaners/Marco_consolidacion/Dimensión 1.xlsx
@@ -471,10 +471,10 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2692,7 +2692,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C88" t="s">
         <v>9</v>
@@ -4148,25 +4148,25 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C144" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D144" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E144" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F144" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G144" t="s">
         <v>15</v>
       </c>
       <c r="H144" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -5500,7 +5500,7 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C196" t="s">
         <v>8</v>
@@ -5509,16 +5509,16 @@
         <v>9</v>
       </c>
       <c r="E196" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F196" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G196" t="s">
         <v>15</v>
       </c>
       <c r="H196" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -6734,13 +6734,13 @@
         <v>11</v>
       </c>
       <c r="F243" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G243" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H243" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="244" spans="1:8">

</xml_diff>

<commit_message>
añadir calificacion de docentes proceso y datos
</commit_message>
<xml_diff>
--- a/utils/cleaners/Marco_consolidacion/Dimensión 1.xlsx
+++ b/utils/cleaners/Marco_consolidacion/Dimensión 1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="15">
   <si>
     <t>Código IE</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>2A</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
   <si>
     <t>1B</t>
@@ -468,13 +465,13 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -494,13 +491,13 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -520,13 +517,13 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -546,13 +543,13 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -572,13 +569,13 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -598,13 +595,13 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -624,13 +621,13 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -650,13 +647,13 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -676,13 +673,13 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -702,13 +699,13 @@
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -728,13 +725,13 @@
         <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -754,13 +751,13 @@
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -780,13 +777,13 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -806,13 +803,13 @@
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -832,13 +829,13 @@
         <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -858,13 +855,13 @@
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -884,13 +881,13 @@
         <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -910,13 +907,13 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -936,13 +933,13 @@
         <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -962,13 +959,13 @@
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -982,19 +979,19 @@
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1014,13 +1011,13 @@
         <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1040,13 +1037,13 @@
         <v>8</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1066,13 +1063,13 @@
         <v>11</v>
       </c>
       <c r="F25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1092,13 +1089,13 @@
         <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1118,13 +1115,13 @@
         <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1144,13 +1141,13 @@
         <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1170,13 +1167,13 @@
         <v>8</v>
       </c>
       <c r="F29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1199,10 +1196,10 @@
         <v>10</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1222,13 +1219,13 @@
         <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1248,13 +1245,13 @@
         <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1274,13 +1271,13 @@
         <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1300,13 +1297,13 @@
         <v>8</v>
       </c>
       <c r="F34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1326,13 +1323,13 @@
         <v>11</v>
       </c>
       <c r="F35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1352,13 +1349,13 @@
         <v>11</v>
       </c>
       <c r="F36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1378,13 +1375,13 @@
         <v>12</v>
       </c>
       <c r="F37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1404,13 +1401,13 @@
         <v>11</v>
       </c>
       <c r="F38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1430,13 +1427,13 @@
         <v>8</v>
       </c>
       <c r="F39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1456,13 +1453,13 @@
         <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1482,13 +1479,13 @@
         <v>11</v>
       </c>
       <c r="F41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1508,13 +1505,13 @@
         <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1534,13 +1531,13 @@
         <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1560,13 +1557,13 @@
         <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1589,10 +1586,10 @@
         <v>10</v>
       </c>
       <c r="G45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1612,13 +1609,13 @@
         <v>8</v>
       </c>
       <c r="F46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1641,10 +1638,10 @@
         <v>10</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1664,13 +1661,13 @@
         <v>8</v>
       </c>
       <c r="F48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1690,13 +1687,13 @@
         <v>8</v>
       </c>
       <c r="F49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1716,13 +1713,13 @@
         <v>8</v>
       </c>
       <c r="F50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1742,13 +1739,13 @@
         <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1768,13 +1765,13 @@
         <v>8</v>
       </c>
       <c r="F52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1794,13 +1791,13 @@
         <v>8</v>
       </c>
       <c r="F53" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G53" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H53" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1820,13 +1817,13 @@
         <v>11</v>
       </c>
       <c r="F54" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G54" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H54" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1846,13 +1843,13 @@
         <v>8</v>
       </c>
       <c r="F55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1872,13 +1869,13 @@
         <v>8</v>
       </c>
       <c r="F56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1898,13 +1895,13 @@
         <v>8</v>
       </c>
       <c r="F57" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G57" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H57" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1924,13 +1921,13 @@
         <v>12</v>
       </c>
       <c r="F58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1950,13 +1947,13 @@
         <v>8</v>
       </c>
       <c r="F59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1976,13 +1973,13 @@
         <v>12</v>
       </c>
       <c r="F60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2002,13 +1999,13 @@
         <v>8</v>
       </c>
       <c r="F61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2028,13 +2025,13 @@
         <v>12</v>
       </c>
       <c r="F62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2054,13 +2051,13 @@
         <v>12</v>
       </c>
       <c r="F63" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G63" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H63" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2080,13 +2077,13 @@
         <v>8</v>
       </c>
       <c r="F64" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G64" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H64" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2106,13 +2103,13 @@
         <v>11</v>
       </c>
       <c r="F65" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G65" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H65" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2132,13 +2129,13 @@
         <v>11</v>
       </c>
       <c r="F66" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G66" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H66" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2158,13 +2155,13 @@
         <v>8</v>
       </c>
       <c r="F67" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G67" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H67" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2184,13 +2181,13 @@
         <v>8</v>
       </c>
       <c r="F68" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G68" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H68" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2210,13 +2207,13 @@
         <v>8</v>
       </c>
       <c r="F69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2236,13 +2233,13 @@
         <v>11</v>
       </c>
       <c r="F70" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G70" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H70" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2262,13 +2259,13 @@
         <v>8</v>
       </c>
       <c r="F71" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G71" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H71" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2288,13 +2285,13 @@
         <v>8</v>
       </c>
       <c r="F72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2314,13 +2311,13 @@
         <v>11</v>
       </c>
       <c r="F73" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G73" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H73" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2340,13 +2337,13 @@
         <v>11</v>
       </c>
       <c r="F74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2366,13 +2363,13 @@
         <v>11</v>
       </c>
       <c r="F75" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G75" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H75" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2392,13 +2389,13 @@
         <v>11</v>
       </c>
       <c r="F76" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G76" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H76" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2418,13 +2415,13 @@
         <v>11</v>
       </c>
       <c r="F77" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G77" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H77" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2444,13 +2441,13 @@
         <v>8</v>
       </c>
       <c r="F78" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G78" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H78" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2470,13 +2467,13 @@
         <v>8</v>
       </c>
       <c r="F79" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G79" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H79" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2496,13 +2493,13 @@
         <v>8</v>
       </c>
       <c r="F80" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G80" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H80" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2522,13 +2519,13 @@
         <v>8</v>
       </c>
       <c r="F81" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G81" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H81" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2548,13 +2545,13 @@
         <v>12</v>
       </c>
       <c r="F82" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G82" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H82" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2574,13 +2571,13 @@
         <v>8</v>
       </c>
       <c r="F83" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G83" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H83" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2600,13 +2597,13 @@
         <v>12</v>
       </c>
       <c r="F84" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G84" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H84" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2626,13 +2623,13 @@
         <v>8</v>
       </c>
       <c r="F85" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G85" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H85" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2652,13 +2649,13 @@
         <v>8</v>
       </c>
       <c r="F86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2678,13 +2675,13 @@
         <v>11</v>
       </c>
       <c r="F87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2704,13 +2701,13 @@
         <v>11</v>
       </c>
       <c r="F88" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G88" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H88" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2733,10 +2730,10 @@
         <v>11</v>
       </c>
       <c r="G89" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H89" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2756,13 +2753,13 @@
         <v>8</v>
       </c>
       <c r="F90" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G90" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H90" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2782,13 +2779,13 @@
         <v>11</v>
       </c>
       <c r="F91" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G91" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H91" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2808,13 +2805,13 @@
         <v>11</v>
       </c>
       <c r="F92" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G92" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H92" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2834,13 +2831,13 @@
         <v>8</v>
       </c>
       <c r="F93" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G93" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H93" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -2860,13 +2857,13 @@
         <v>11</v>
       </c>
       <c r="F94" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G94" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H94" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2886,13 +2883,13 @@
         <v>8</v>
       </c>
       <c r="F95" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G95" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H95" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -2912,13 +2909,13 @@
         <v>11</v>
       </c>
       <c r="F96" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G96" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H96" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2938,13 +2935,13 @@
         <v>8</v>
       </c>
       <c r="F97" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G97" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H97" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -2964,13 +2961,13 @@
         <v>8</v>
       </c>
       <c r="F98" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G98" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H98" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -2990,13 +2987,13 @@
         <v>11</v>
       </c>
       <c r="F99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H99" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -3016,13 +3013,13 @@
         <v>8</v>
       </c>
       <c r="F100" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G100" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H100" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -3042,13 +3039,13 @@
         <v>8</v>
       </c>
       <c r="F101" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G101" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H101" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="102" spans="1:8">
@@ -3068,13 +3065,13 @@
         <v>8</v>
       </c>
       <c r="F102" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G102" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H102" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -3097,10 +3094,10 @@
         <v>11</v>
       </c>
       <c r="G103" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H103" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -3123,10 +3120,10 @@
         <v>11</v>
       </c>
       <c r="G104" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H104" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:8">
@@ -3146,13 +3143,13 @@
         <v>12</v>
       </c>
       <c r="F105" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G105" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H105" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:8">
@@ -3172,13 +3169,13 @@
         <v>12</v>
       </c>
       <c r="F106" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G106" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H106" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="107" spans="1:8">
@@ -3198,13 +3195,13 @@
         <v>8</v>
       </c>
       <c r="F107" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G107" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H107" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -3224,13 +3221,13 @@
         <v>11</v>
       </c>
       <c r="F108" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G108" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H108" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -3250,13 +3247,13 @@
         <v>8</v>
       </c>
       <c r="F109" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G109" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H109" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -3276,13 +3273,13 @@
         <v>8</v>
       </c>
       <c r="F110" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G110" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H110" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -3302,13 +3299,13 @@
         <v>11</v>
       </c>
       <c r="F111" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G111" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H111" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -3328,13 +3325,13 @@
         <v>11</v>
       </c>
       <c r="F112" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G112" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H112" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:8">
@@ -3354,13 +3351,13 @@
         <v>11</v>
       </c>
       <c r="F113" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G113" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H113" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:8">
@@ -3380,13 +3377,13 @@
         <v>8</v>
       </c>
       <c r="F114" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G114" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H114" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:8">
@@ -3406,13 +3403,13 @@
         <v>12</v>
       </c>
       <c r="F115" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G115" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H115" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:8">
@@ -3432,13 +3429,13 @@
         <v>11</v>
       </c>
       <c r="F116" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G116" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H116" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:8">
@@ -3458,13 +3455,13 @@
         <v>8</v>
       </c>
       <c r="F117" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G117" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H117" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:8">
@@ -3484,13 +3481,13 @@
         <v>8</v>
       </c>
       <c r="F118" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G118" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H118" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:8">
@@ -3510,13 +3507,13 @@
         <v>8</v>
       </c>
       <c r="F119" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G119" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H119" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:8">
@@ -3536,13 +3533,13 @@
         <v>12</v>
       </c>
       <c r="F120" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G120" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H120" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:8">
@@ -3562,13 +3559,13 @@
         <v>8</v>
       </c>
       <c r="F121" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G121" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H121" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:8">
@@ -3588,13 +3585,13 @@
         <v>8</v>
       </c>
       <c r="F122" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G122" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H122" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -3614,13 +3611,13 @@
         <v>11</v>
       </c>
       <c r="F123" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G123" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H123" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:8">
@@ -3640,13 +3637,13 @@
         <v>12</v>
       </c>
       <c r="F124" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G124" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H124" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -3666,13 +3663,13 @@
         <v>11</v>
       </c>
       <c r="F125" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G125" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H125" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -3692,13 +3689,13 @@
         <v>11</v>
       </c>
       <c r="F126" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G126" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H126" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:8">
@@ -3718,13 +3715,13 @@
         <v>11</v>
       </c>
       <c r="F127" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G127" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H127" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:8">
@@ -3744,13 +3741,13 @@
         <v>11</v>
       </c>
       <c r="F128" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G128" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H128" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -3770,13 +3767,13 @@
         <v>11</v>
       </c>
       <c r="F129" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G129" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H129" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -3796,13 +3793,13 @@
         <v>8</v>
       </c>
       <c r="F130" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G130" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H130" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:8">
@@ -3822,13 +3819,13 @@
         <v>11</v>
       </c>
       <c r="F131" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G131" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H131" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:8">
@@ -3848,13 +3845,13 @@
         <v>11</v>
       </c>
       <c r="F132" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G132" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H132" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:8">
@@ -3874,13 +3871,13 @@
         <v>8</v>
       </c>
       <c r="F133" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G133" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H133" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -3900,13 +3897,13 @@
         <v>11</v>
       </c>
       <c r="F134" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G134" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H134" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:8">
@@ -3926,13 +3923,13 @@
         <v>11</v>
       </c>
       <c r="F135" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G135" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H135" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:8">
@@ -3952,13 +3949,13 @@
         <v>11</v>
       </c>
       <c r="F136" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G136" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H136" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -3978,13 +3975,13 @@
         <v>8</v>
       </c>
       <c r="F137" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G137" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H137" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -4004,13 +4001,13 @@
         <v>8</v>
       </c>
       <c r="F138" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G138" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H138" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:8">
@@ -4030,13 +4027,13 @@
         <v>11</v>
       </c>
       <c r="F139" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G139" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H139" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:8">
@@ -4056,13 +4053,13 @@
         <v>8</v>
       </c>
       <c r="F140" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G140" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H140" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -4082,13 +4079,13 @@
         <v>8</v>
       </c>
       <c r="F141" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G141" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H141" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:8">
@@ -4108,13 +4105,13 @@
         <v>8</v>
       </c>
       <c r="F142" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G142" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H142" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:8">
@@ -4134,13 +4131,13 @@
         <v>11</v>
       </c>
       <c r="F143" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G143" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H143" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:8">
@@ -4160,13 +4157,13 @@
         <v>12</v>
       </c>
       <c r="F144" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G144" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H144" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:8">
@@ -4186,13 +4183,13 @@
         <v>12</v>
       </c>
       <c r="F145" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G145" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H145" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:8">
@@ -4212,13 +4209,13 @@
         <v>8</v>
       </c>
       <c r="F146" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G146" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H146" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:8">
@@ -4238,13 +4235,13 @@
         <v>11</v>
       </c>
       <c r="F147" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G147" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H147" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:8">
@@ -4264,13 +4261,13 @@
         <v>8</v>
       </c>
       <c r="F148" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G148" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H148" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" spans="1:8">
@@ -4290,13 +4287,13 @@
         <v>11</v>
       </c>
       <c r="F149" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G149" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H149" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:8">
@@ -4316,13 +4313,13 @@
         <v>12</v>
       </c>
       <c r="F150" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G150" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H150" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" spans="1:8">
@@ -4342,13 +4339,13 @@
         <v>8</v>
       </c>
       <c r="F151" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G151" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H151" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="152" spans="1:8">
@@ -4368,13 +4365,13 @@
         <v>8</v>
       </c>
       <c r="F152" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G152" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H152" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="153" spans="1:8">
@@ -4394,13 +4391,13 @@
         <v>8</v>
       </c>
       <c r="F153" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G153" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H153" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="1:8">
@@ -4420,13 +4417,13 @@
         <v>11</v>
       </c>
       <c r="F154" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G154" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H154" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:8">
@@ -4449,10 +4446,10 @@
         <v>10</v>
       </c>
       <c r="G155" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H155" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="156" spans="1:8">
@@ -4472,13 +4469,13 @@
         <v>12</v>
       </c>
       <c r="F156" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G156" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H156" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:8">
@@ -4498,13 +4495,13 @@
         <v>8</v>
       </c>
       <c r="F157" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G157" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H157" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:8">
@@ -4524,13 +4521,13 @@
         <v>11</v>
       </c>
       <c r="F158" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G158" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H158" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:8">
@@ -4550,13 +4547,13 @@
         <v>8</v>
       </c>
       <c r="F159" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G159" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H159" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160" spans="1:8">
@@ -4576,13 +4573,13 @@
         <v>8</v>
       </c>
       <c r="F160" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G160" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H160" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:8">
@@ -4602,13 +4599,13 @@
         <v>8</v>
       </c>
       <c r="F161" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G161" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H161" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="162" spans="1:8">
@@ -4628,13 +4625,13 @@
         <v>8</v>
       </c>
       <c r="F162" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G162" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H162" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:8">
@@ -4654,13 +4651,13 @@
         <v>8</v>
       </c>
       <c r="F163" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G163" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H163" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="164" spans="1:8">
@@ -4683,10 +4680,10 @@
         <v>11</v>
       </c>
       <c r="G164" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H164" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:8">
@@ -4709,10 +4706,10 @@
         <v>11</v>
       </c>
       <c r="G165" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H165" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:8">
@@ -4735,10 +4732,10 @@
         <v>10</v>
       </c>
       <c r="G166" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H166" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="167" spans="1:8">
@@ -4761,10 +4758,10 @@
         <v>11</v>
       </c>
       <c r="G167" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H167" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -4784,13 +4781,13 @@
         <v>11</v>
       </c>
       <c r="F168" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G168" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H168" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:8">
@@ -4813,10 +4810,10 @@
         <v>11</v>
       </c>
       <c r="G169" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H169" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="170" spans="1:8">
@@ -4836,13 +4833,13 @@
         <v>8</v>
       </c>
       <c r="F170" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G170" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H170" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:8">
@@ -4862,13 +4859,13 @@
         <v>8</v>
       </c>
       <c r="F171" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G171" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H171" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:8">
@@ -4888,13 +4885,13 @@
         <v>8</v>
       </c>
       <c r="F172" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G172" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H172" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="173" spans="1:8">
@@ -4914,13 +4911,13 @@
         <v>8</v>
       </c>
       <c r="F173" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G173" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H173" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -4943,10 +4940,10 @@
         <v>10</v>
       </c>
       <c r="G174" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H174" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:8">
@@ -4966,13 +4963,13 @@
         <v>8</v>
       </c>
       <c r="F175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G175" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -4995,10 +4992,10 @@
         <v>10</v>
       </c>
       <c r="G176" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H176" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -5018,13 +5015,13 @@
         <v>11</v>
       </c>
       <c r="F177" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G177" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H177" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -5044,13 +5041,13 @@
         <v>8</v>
       </c>
       <c r="F178" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G178" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H178" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -5070,13 +5067,13 @@
         <v>8</v>
       </c>
       <c r="F179" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G179" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H179" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -5096,13 +5093,13 @@
         <v>11</v>
       </c>
       <c r="F180" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G180" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H180" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -5122,13 +5119,13 @@
         <v>11</v>
       </c>
       <c r="F181" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G181" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H181" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -5148,13 +5145,13 @@
         <v>8</v>
       </c>
       <c r="F182" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G182" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H182" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -5174,13 +5171,13 @@
         <v>11</v>
       </c>
       <c r="F183" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G183" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H183" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -5200,13 +5197,13 @@
         <v>8</v>
       </c>
       <c r="F184" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G184" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H184" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -5226,13 +5223,13 @@
         <v>8</v>
       </c>
       <c r="F185" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G185" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H185" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -5252,13 +5249,13 @@
         <v>11</v>
       </c>
       <c r="F186" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G186" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H186" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -5281,10 +5278,10 @@
         <v>10</v>
       </c>
       <c r="G187" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H187" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -5304,13 +5301,13 @@
         <v>8</v>
       </c>
       <c r="F188" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G188" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H188" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -5333,10 +5330,10 @@
         <v>11</v>
       </c>
       <c r="G189" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H189" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -5356,13 +5353,13 @@
         <v>8</v>
       </c>
       <c r="F190" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G190" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H190" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -5382,13 +5379,13 @@
         <v>8</v>
       </c>
       <c r="F191" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G191" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H191" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -5408,13 +5405,13 @@
         <v>11</v>
       </c>
       <c r="F192" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G192" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H192" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -5434,13 +5431,13 @@
         <v>8</v>
       </c>
       <c r="F193" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G193" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H193" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:8">
@@ -5460,13 +5457,13 @@
         <v>8</v>
       </c>
       <c r="F194" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G194" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H194" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:8">
@@ -5486,13 +5483,13 @@
         <v>11</v>
       </c>
       <c r="F195" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G195" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H195" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:8">
@@ -5512,13 +5509,13 @@
         <v>11</v>
       </c>
       <c r="F196" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G196" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H196" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:8">
@@ -5535,16 +5532,16 @@
         <v>11</v>
       </c>
       <c r="E197" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F197" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G197" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H197" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:8">
@@ -5564,13 +5561,13 @@
         <v>8</v>
       </c>
       <c r="F198" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G198" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H198" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:8">
@@ -5590,13 +5587,13 @@
         <v>11</v>
       </c>
       <c r="F199" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G199" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H199" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="200" spans="1:8">
@@ -5616,13 +5613,13 @@
         <v>8</v>
       </c>
       <c r="F200" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G200" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H200" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -5642,13 +5639,13 @@
         <v>11</v>
       </c>
       <c r="F201" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G201" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H201" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="202" spans="1:8">
@@ -5668,13 +5665,13 @@
         <v>11</v>
       </c>
       <c r="F202" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G202" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H202" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -5694,13 +5691,13 @@
         <v>12</v>
       </c>
       <c r="F203" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G203" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H203" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="204" spans="1:8">
@@ -5720,13 +5717,13 @@
         <v>11</v>
       </c>
       <c r="F204" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G204" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H204" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="205" spans="1:8">
@@ -5746,13 +5743,13 @@
         <v>8</v>
       </c>
       <c r="F205" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G205" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H205" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="206" spans="1:8">
@@ -5772,13 +5769,13 @@
         <v>12</v>
       </c>
       <c r="F206" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G206" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H206" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="207" spans="1:8">
@@ -5801,10 +5798,10 @@
         <v>10</v>
       </c>
       <c r="G207" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H207" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="208" spans="1:8">
@@ -5824,13 +5821,13 @@
         <v>8</v>
       </c>
       <c r="F208" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G208" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H208" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="209" spans="1:8">
@@ -5850,13 +5847,13 @@
         <v>12</v>
       </c>
       <c r="F209" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G209" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H209" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="210" spans="1:8">
@@ -5876,13 +5873,13 @@
         <v>8</v>
       </c>
       <c r="F210" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G210" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H210" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -5902,13 +5899,13 @@
         <v>8</v>
       </c>
       <c r="F211" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G211" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H211" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -5928,13 +5925,13 @@
         <v>11</v>
       </c>
       <c r="F212" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G212" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H212" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="213" spans="1:8">
@@ -5954,13 +5951,13 @@
         <v>8</v>
       </c>
       <c r="F213" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G213" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H213" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="214" spans="1:8">
@@ -5983,10 +5980,10 @@
         <v>10</v>
       </c>
       <c r="G214" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H214" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="215" spans="1:8">
@@ -6009,10 +6006,10 @@
         <v>10</v>
       </c>
       <c r="G215" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H215" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="216" spans="1:8">
@@ -6032,13 +6029,13 @@
         <v>8</v>
       </c>
       <c r="F216" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G216" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H216" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="217" spans="1:8">
@@ -6058,13 +6055,13 @@
         <v>12</v>
       </c>
       <c r="F217" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G217" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H217" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -6084,13 +6081,13 @@
         <v>8</v>
       </c>
       <c r="F218" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G218" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H218" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -6110,13 +6107,13 @@
         <v>8</v>
       </c>
       <c r="F219" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G219" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H219" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="220" spans="1:8">
@@ -6136,13 +6133,13 @@
         <v>11</v>
       </c>
       <c r="F220" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G220" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H220" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="221" spans="1:8">
@@ -6162,13 +6159,13 @@
         <v>8</v>
       </c>
       <c r="F221" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G221" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H221" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="222" spans="1:8">
@@ -6188,13 +6185,13 @@
         <v>8</v>
       </c>
       <c r="F222" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G222" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H222" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -6214,13 +6211,13 @@
         <v>8</v>
       </c>
       <c r="F223" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G223" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H223" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="224" spans="1:8">
@@ -6240,13 +6237,13 @@
         <v>11</v>
       </c>
       <c r="F224" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G224" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H224" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="225" spans="1:8">
@@ -6266,13 +6263,13 @@
         <v>8</v>
       </c>
       <c r="F225" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G225" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H225" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="226" spans="1:8">
@@ -6295,10 +6292,10 @@
         <v>10</v>
       </c>
       <c r="G226" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H226" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="227" spans="1:8">
@@ -6318,13 +6315,13 @@
         <v>11</v>
       </c>
       <c r="F227" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G227" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H227" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="228" spans="1:8">
@@ -6341,16 +6338,16 @@
         <v>8</v>
       </c>
       <c r="E228" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F228" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G228" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H228" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="229" spans="1:8">
@@ -6370,13 +6367,13 @@
         <v>11</v>
       </c>
       <c r="F229" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G229" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H229" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -6396,13 +6393,13 @@
         <v>8</v>
       </c>
       <c r="F230" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G230" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H230" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="231" spans="1:8">
@@ -6422,13 +6419,13 @@
         <v>11</v>
       </c>
       <c r="F231" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G231" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H231" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="232" spans="1:8">
@@ -6448,13 +6445,13 @@
         <v>11</v>
       </c>
       <c r="F232" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G232" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H232" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="233" spans="1:8">
@@ -6474,13 +6471,13 @@
         <v>8</v>
       </c>
       <c r="F233" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G233" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H233" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -6503,10 +6500,10 @@
         <v>10</v>
       </c>
       <c r="G234" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H234" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -6529,10 +6526,10 @@
         <v>10</v>
       </c>
       <c r="G235" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H235" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="236" spans="1:8">
@@ -6552,13 +6549,13 @@
         <v>11</v>
       </c>
       <c r="F236" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G236" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H236" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="237" spans="1:8">
@@ -6578,13 +6575,13 @@
         <v>8</v>
       </c>
       <c r="F237" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G237" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H237" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -6604,13 +6601,13 @@
         <v>8</v>
       </c>
       <c r="F238" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G238" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H238" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="239" spans="1:8">
@@ -6630,13 +6627,13 @@
         <v>8</v>
       </c>
       <c r="F239" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G239" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H239" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -6656,13 +6653,13 @@
         <v>11</v>
       </c>
       <c r="F240" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G240" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H240" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="241" spans="1:8">
@@ -6682,13 +6679,13 @@
         <v>8</v>
       </c>
       <c r="F241" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G241" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H241" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="242" spans="1:8">
@@ -6708,13 +6705,13 @@
         <v>8</v>
       </c>
       <c r="F242" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G242" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H242" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="243" spans="1:8">
@@ -6734,13 +6731,13 @@
         <v>11</v>
       </c>
       <c r="F243" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G243" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H243" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="244" spans="1:8">
@@ -6757,16 +6754,16 @@
         <v>9</v>
       </c>
       <c r="E244" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F244" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G244" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H244" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="245" spans="1:8">
@@ -6786,13 +6783,13 @@
         <v>8</v>
       </c>
       <c r="F245" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G245" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H245" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -6812,13 +6809,13 @@
         <v>11</v>
       </c>
       <c r="F246" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G246" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H246" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="247" spans="1:8">
@@ -6838,13 +6835,13 @@
         <v>8</v>
       </c>
       <c r="F247" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G247" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H247" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="248" spans="1:8">
@@ -6864,13 +6861,13 @@
         <v>8</v>
       </c>
       <c r="F248" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G248" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H248" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="249" spans="1:8">
@@ -6890,13 +6887,13 @@
         <v>11</v>
       </c>
       <c r="F249" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G249" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H249" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="250" spans="1:8">
@@ -6919,10 +6916,10 @@
         <v>10</v>
       </c>
       <c r="G250" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H250" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="251" spans="1:8">
@@ -6942,13 +6939,13 @@
         <v>8</v>
       </c>
       <c r="F251" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G251" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H251" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="252" spans="1:8">
@@ -6968,13 +6965,13 @@
         <v>8</v>
       </c>
       <c r="F252" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G252" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H252" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="253" spans="1:8">
@@ -6994,13 +6991,13 @@
         <v>8</v>
       </c>
       <c r="F253" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G253" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H253" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>